<commit_message>
test_Sauce_Optioanl.py file made with constant and .xlsx file
</commit_message>
<xml_diff>
--- a/data/login.xlsx
+++ b/data/login.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/recepodemis/Desktop/gitRepo/Pytest-SauceDemo-Automation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F6275E2-E2F9-B541-9399-D40ED305FD04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EA0949-C78B-3C45-9700-A8BD82A6E9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17880" yWindow="1500" windowWidth="12940" windowHeight="17440" activeTab="2" xr2:uid="{040E23C6-A0B4-314D-9355-D8BCD9990D63}"/>
+    <workbookView xWindow="17880" yWindow="1500" windowWidth="12940" windowHeight="17440" activeTab="3" xr2:uid="{040E23C6-A0B4-314D-9355-D8BCD9990D63}"/>
   </bookViews>
   <sheets>
     <sheet name="only_username" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -57,6 +57,15 @@
   </si>
   <si>
     <t>locked_out_user</t>
+  </si>
+  <si>
+    <t>testrecep</t>
+  </si>
+  <si>
+    <t>test_password</t>
+  </si>
+  <si>
+    <t>deneme</t>
   </si>
 </sst>
 </file>
@@ -464,10 +473,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C189B8-A9DE-0F4A-BD0A-E4C168BF9202}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -482,10 +491,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -497,7 +522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE659FB6-B52B-A046-BC65-6B4BEDDE03ED}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>